<commit_message>
update new verision V1.2 to V1.3 for RTM
add new tracebility metrix from Foodies_RTM_044 to Foodies_RTM_049
</commit_message>
<xml_diff>
--- a/Foodies_RTM.xlsx
+++ b/Foodies_RTM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -63,102 +63,9 @@
     <t>create RTM Table</t>
   </si>
   <si>
-    <t xml:space="preserve">add SIQ , SRS , CRS </t>
-  </si>
-  <si>
-    <t>Foodie_RTM_001</t>
-  </si>
-  <si>
     <t>Foodies_CRS_001</t>
   </si>
   <si>
-    <t>Foodie_RTM_002</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_003</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_004</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_005</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_006</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_007</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_008</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_009</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_010</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_011</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_012</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_013</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_014</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_015</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_016</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_017</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_018</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_019</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_020</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_021</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_022</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_023</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_024</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_025</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_026</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_027</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_028</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_029</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_030</t>
-  </si>
-  <si>
     <t>Foodies_SRS_001</t>
   </si>
   <si>
@@ -309,48 +216,9 @@
     <t>Foodies_SRS_036</t>
   </si>
   <si>
-    <t>Foodie_RTM_031</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_032</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_033</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_034</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_035</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_036</t>
-  </si>
-  <si>
     <t>Foodies_SIQ_015</t>
   </si>
   <si>
-    <t>Foodie_RTM_037</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_038</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_039</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_040</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_041</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_042</t>
-  </si>
-  <si>
-    <t>Foodie_RTM_043</t>
-  </si>
-  <si>
     <t>Foodies_SRS_037</t>
   </si>
   <si>
@@ -406,6 +274,207 @@
   </si>
   <si>
     <t>edit columns names</t>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_001</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_002</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_003</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_004</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_005</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_006</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_007</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_008</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_009</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_010</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_011</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_012</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_013</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_014</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_015</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_016</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_017</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_018</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_019</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_020</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_021</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_022</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_023</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_024</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_025</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_026</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_027</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_028</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_029</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_030</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_031</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_032</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_033</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_034</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_035</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_036</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_037</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_038</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_039</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_040</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_041</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_042</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add SIQ , SRS , CRS  from Foodies_RTM_001 to Foodies_RTM_043  </t>
+  </si>
+  <si>
+    <t>Foodies_RTM_044</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_045</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_046</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_047</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_048</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_049</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_044</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_045</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_046</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_047</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_048</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_049</t>
+  </si>
+  <si>
+    <t>add SRS , CRS from Foodies_RTM_044 to Foodies_RTM_045</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_019</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_020</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_021</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_022</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_023</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_024</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_003 , Foodies_SIQ_025</t>
+  </si>
+  <si>
+    <t>Foodies_SIQ_025</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -500,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -522,6 +591,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,8 +674,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H47" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:H47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H56" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:H56"/>
   <tableColumns count="8">
     <tableColumn id="1" name="ID" dataDxfId="15"/>
     <tableColumn id="2" name="Business Requirment ID" dataDxfId="14"/>
@@ -914,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
@@ -960,16 +1038,16 @@
     </row>
     <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -978,34 +1056,34 @@
     </row>
     <row r="3" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>68</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1014,16 +1092,16 @@
     </row>
     <row r="5" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1032,16 +1110,16 @@
     </row>
     <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1050,16 +1128,16 @@
     </row>
     <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1068,15 +1146,17 @@
     </row>
     <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1084,16 +1164,16 @@
     </row>
     <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1102,13 +1182,13 @@
     </row>
     <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1118,13 +1198,13 @@
     </row>
     <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1134,13 +1214,13 @@
     </row>
     <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1150,16 +1230,16 @@
     </row>
     <row r="13" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1168,16 +1248,16 @@
     </row>
     <row r="14" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1186,16 +1266,16 @@
     </row>
     <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1204,16 +1284,16 @@
     </row>
     <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1222,13 +1302,13 @@
     </row>
     <row r="17" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1238,16 +1318,16 @@
     </row>
     <row r="18" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1256,16 +1336,16 @@
     </row>
     <row r="19" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1274,16 +1354,16 @@
     </row>
     <row r="20" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1292,16 +1372,16 @@
     </row>
     <row r="21" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1310,16 +1390,16 @@
     </row>
     <row r="22" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1328,16 +1408,16 @@
     </row>
     <row r="23" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="C23" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1346,16 +1426,16 @@
     </row>
     <row r="24" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1364,16 +1444,16 @@
     </row>
     <row r="25" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1382,16 +1462,16 @@
     </row>
     <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1400,13 +1480,13 @@
     </row>
     <row r="27" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1416,13 +1496,13 @@
     </row>
     <row r="28" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1432,13 +1512,13 @@
     </row>
     <row r="29" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1448,13 +1528,13 @@
     </row>
     <row r="30" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1464,13 +1544,13 @@
     </row>
     <row r="31" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1480,13 +1560,13 @@
     </row>
     <row r="32" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1496,13 +1576,13 @@
     </row>
     <row r="33" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1512,13 +1592,13 @@
     </row>
     <row r="34" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -1528,13 +1608,13 @@
     </row>
     <row r="35" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1544,13 +1624,13 @@
     </row>
     <row r="36" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -1560,16 +1640,16 @@
     </row>
     <row r="37" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1578,16 +1658,16 @@
     </row>
     <row r="38" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1596,16 +1676,16 @@
     </row>
     <row r="39" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1614,16 +1694,16 @@
     </row>
     <row r="40" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1632,13 +1712,13 @@
     </row>
     <row r="41" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="3"/>
@@ -1648,13 +1728,13 @@
     </row>
     <row r="42" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="3"/>
@@ -1664,16 +1744,16 @@
     </row>
     <row r="43" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1682,51 +1762,189 @@
     </row>
     <row r="44" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+    <row r="45" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+    <row r="46" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+    <row r="47" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1759,19 +1977,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1992,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,12 +2249,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -2044,12 +2262,23 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update new verision ( V1.4 ) for RTM
add new row Foodies_RTM_050
</commit_message>
<xml_diff>
--- a/Foodies_RTM.xlsx
+++ b/Foodies_RTM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="157">
   <si>
     <t>ID</t>
   </si>
@@ -447,9 +447,6 @@
     <t>Foodies_SRS_049</t>
   </si>
   <si>
-    <t>add SRS , CRS from Foodies_RTM_044 to Foodies_RTM_045</t>
-  </si>
-  <si>
     <t>Foodies_SIQ_019</t>
   </si>
   <si>
@@ -475,6 +472,21 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Foodies_SRS_050</t>
+  </si>
+  <si>
+    <t>Foodies_RTM_050</t>
+  </si>
+  <si>
+    <t>V1.4</t>
+  </si>
+  <si>
+    <t>add SRS , CRS , SIQ from Foodies_RTM_044 to Foodies_RTM_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add SRS , CRS , SIQ for Foodies_RTM_050 </t>
   </si>
 </sst>
 </file>
@@ -995,7 +1007,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1095,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1155,7 +1167,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1783,13 +1795,13 @@
         <v>131</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>137</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1801,13 +1813,13 @@
         <v>132</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1819,13 +1831,13 @@
         <v>133</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>139</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -1837,13 +1849,13 @@
         <v>134</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>140</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -1855,13 +1867,13 @@
         <v>135</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>141</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -1873,13 +1885,13 @@
         <v>136</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>142</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -1887,10 +1899,18 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -1948,8 +1968,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2210,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,9 +2297,20 @@
         <v>86</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>